<commit_message>
Actualización automática desde Jupyter
</commit_message>
<xml_diff>
--- a/paraderos_ruta_80JQ_R.xlsx
+++ b/paraderos_ruta_80JQ_R.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minbo\Desktop\Trabajo FINAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexf\OneDrive\Escritorio\Trabajo Simu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D59D98-997D-49AB-9E88-BB1ED85B263D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83214304-84E8-4369-BA98-84C5F6E068F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,9 +34,6 @@
     <t>lon</t>
   </si>
   <si>
-    <t>JQ_R</t>
-  </si>
-  <si>
     <t>Pedro Montt Esq La Marina Sur</t>
   </si>
   <si>
@@ -602,6 +599,9 @@
   </si>
   <si>
     <t>Tegualda Esq Calle1 Poniente</t>
+  </si>
+  <si>
+    <t>80JQ_R</t>
   </si>
 </sst>
 </file>
@@ -662,7 +662,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,10 +996,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" s="2">
         <v>-36.724224999999997</v>
@@ -1010,24 +1010,24 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>-36.810496999999998</v>
@@ -1038,24 +1038,24 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2">
         <v>-36.724080000000001</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>-36.723897000000001</v>
@@ -1080,10 +1080,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
         <v>-36.721406999999999</v>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2">
         <v>-36.717508000000002</v>
@@ -1108,10 +1108,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="2">
         <v>-36.827016999999998</v>
@@ -1122,10 +1122,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2">
         <v>-36.714216</v>
@@ -1136,10 +1136,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="2">
         <v>-36.713135999999999</v>
@@ -1150,52 +1150,52 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2">
         <v>-36.718020000000003</v>
@@ -1206,38 +1206,38 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2">
         <v>-36.724558000000002</v>
@@ -1248,38 +1248,38 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2">
         <v>-36.732306999999999</v>
@@ -1290,10 +1290,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="2">
         <v>-36.7346</v>
@@ -1304,94 +1304,94 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" s="2">
         <v>-36.752979000000003</v>
@@ -1402,24 +1402,24 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" s="2">
         <v>-36.758346000000003</v>
@@ -1430,24 +1430,24 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="2">
         <v>-36.764038999999997</v>
@@ -1458,38 +1458,38 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B36" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="2">
         <v>-36.774422000000001</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="2">
         <v>-36.781312999999997</v>
@@ -1514,10 +1514,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="2">
         <v>-36.791088999999999</v>
@@ -1528,10 +1528,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="2">
         <v>-36.933020999999997</v>
@@ -1542,10 +1542,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" s="2">
         <v>-36.825887999999999</v>
@@ -1556,38 +1556,38 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B42" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="2">
         <v>-36.810496999999998</v>
@@ -1598,10 +1598,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" s="2">
         <v>-36.812556999999998</v>
@@ -1612,24 +1612,24 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="2">
         <v>-36.816608000000002</v>
@@ -1640,24 +1640,24 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="2">
         <v>-36.712176999999997</v>
@@ -1668,10 +1668,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" s="2">
         <v>-36.822014000000003</v>
@@ -1682,94 +1682,94 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B51" t="s">
+        <v>76</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B53" t="s">
+        <v>80</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B55" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D55" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D56" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B57" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C57" s="2">
         <v>-36.834162999999997</v>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B58" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C58" s="2">
         <v>-36.836193999999999</v>
@@ -1794,10 +1794,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C59" s="2">
         <v>-36.836193999999999</v>
@@ -1808,66 +1808,66 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="D60" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B61" t="s">
+        <v>92</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D61" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="D62" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B63" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="D63" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C64" s="2">
         <v>-36.850748000000003</v>
@@ -1878,10 +1878,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" s="2">
         <v>-36.852846999999997</v>
@@ -1892,10 +1892,10 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C66" s="2">
         <v>-36.855654999999999</v>
@@ -1906,10 +1906,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C67" s="2">
         <v>-36.865524000000001</v>
@@ -1920,10 +1920,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C68" s="2">
         <v>-36.867258999999997</v>
@@ -1934,10 +1934,10 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C69" s="2">
         <v>-36.870206000000003</v>
@@ -1948,10 +1948,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B70" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C70" s="2">
         <v>-36.874237999999998</v>
@@ -1962,10 +1962,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C71" s="2">
         <v>-36.880273000000003</v>
@@ -1976,10 +1976,10 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72" s="2">
         <v>-36.885064999999997</v>
@@ -1990,10 +1990,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C73" s="2">
         <v>-36.890453999999998</v>
@@ -2004,10 +2004,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74" s="2">
         <v>-36.897931999999997</v>
@@ -2018,24 +2018,24 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B75" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C75" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="D75" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B76" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C76" s="2">
         <v>-36.901287000000004</v>
@@ -2046,10 +2046,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C77" s="2">
         <v>-36.905025000000002</v>
@@ -2060,24 +2060,24 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="D78" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B79" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C79" s="2">
         <v>-36.933020999999997</v>
@@ -2088,24 +2088,24 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B80" t="s">
+        <v>116</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C81" s="2">
         <v>-36.915644</v>
@@ -2116,80 +2116,80 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B82" t="s">
+        <v>119</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>121</v>
-      </c>
       <c r="D82" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B83" t="s">
+        <v>121</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="D83" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B84" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="D84" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B85" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C85" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B86" t="s">
+        <v>127</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>129</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B87" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C87" s="2">
         <v>-36.931158000000003</v>
@@ -2200,66 +2200,66 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B88" t="s">
+        <v>130</v>
+      </c>
+      <c r="C88" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C88" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="D88" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B89" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C89" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="D89" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B90" t="s">
+        <v>134</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C90" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="D90" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B91" t="s">
+        <v>136</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C91" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="D91" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C92" s="2">
         <v>-36.945196000000003</v>
@@ -2270,10 +2270,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C93" s="2">
         <v>-36.947339999999997</v>
@@ -2284,94 +2284,94 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B94" t="s">
+        <v>140</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="D94" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B95" t="s">
+        <v>142</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>144</v>
-      </c>
       <c r="D95" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B96" t="s">
+        <v>144</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="D96" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B97" t="s">
+        <v>146</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C97" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D97" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
+        <v>148</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="D98" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B99" t="s">
+        <v>150</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="D99" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B100" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C100" s="2">
         <v>-36.967351999999998</v>
@@ -2382,10 +2382,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B101" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C101" s="2">
         <v>-36.964222999999997</v>
@@ -2396,10 +2396,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B102" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C102" s="2">
         <v>-36.964174</v>
@@ -2410,10 +2410,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C103" s="2">
         <v>-36.964415000000002</v>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C104" s="2">
         <v>-36.969039000000002</v>
@@ -2438,10 +2438,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B105" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C105" s="2">
         <v>-36.969414</v>
@@ -2452,10 +2452,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B106" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C106" s="2">
         <v>-36.970582</v>
@@ -2466,24 +2466,24 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B107" t="s">
+        <v>159</v>
+      </c>
+      <c r="C107" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C107" s="2" t="s">
-        <v>161</v>
-      </c>
       <c r="D107" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C108" s="2">
         <v>-36.980238</v>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C109" s="2">
         <v>-36.974342999999998</v>
@@ -2508,10 +2508,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B110" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C110" s="2">
         <v>-36.865524000000001</v>
@@ -2522,24 +2522,24 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B111" t="s">
+        <v>164</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C111" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="D111" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B112" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C112" s="2">
         <v>-36.974348999999997</v>
@@ -2550,10 +2550,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B113" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C113" s="2">
         <v>-36.97298</v>
@@ -2564,10 +2564,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B114" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C114" s="2">
         <v>-36.919297999999998</v>
@@ -2578,38 +2578,38 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B115" t="s">
+        <v>169</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="D115" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B116" t="s">
+        <v>171</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C116" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="D116" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B117" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C117" s="2">
         <v>-36.968994000000002</v>
@@ -2620,10 +2620,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B118" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C118" s="2">
         <v>-36.968379520455002</v>
@@ -2634,24 +2634,24 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B119" t="s">
+        <v>175</v>
+      </c>
+      <c r="C119" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>177</v>
-      </c>
       <c r="D119" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B120" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C120" s="2">
         <v>-36.966679999999997</v>
@@ -2662,38 +2662,38 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B121" t="s">
+        <v>178</v>
+      </c>
+      <c r="C121" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="D121" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B122" t="s">
+        <v>180</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="D122" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B123" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C123" s="2">
         <v>-36.964388999999997</v>
@@ -2704,24 +2704,24 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B124" t="s">
+        <v>183</v>
+      </c>
+      <c r="C124" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="D124" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B125" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C125" s="2">
         <v>-36.961666999999998</v>
@@ -2732,10 +2732,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B126" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C126" s="2">
         <v>-36.963075000000003</v>
@@ -2746,38 +2746,38 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B127" t="s">
+        <v>187</v>
+      </c>
+      <c r="C127" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="D127" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B128" t="s">
+        <v>189</v>
+      </c>
+      <c r="C128" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>191</v>
-      </c>
       <c r="D128" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B129" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C129" s="2">
         <v>-36.968237999999999</v>
@@ -2788,10 +2788,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>4</v>
+        <v>193</v>
       </c>
       <c r="B130" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C130" s="2">
         <v>-36.970067999999998</v>

</xml_diff>